<commit_message>
test_urls: fix Czech Republic
</commit_message>
<xml_diff>
--- a/manual/tests_urls.xlsx
+++ b/manual/tests_urls.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="845" uniqueCount="467">
   <si>
     <t>country</t>
   </si>
@@ -2820,8 +2820,8 @@
       <c r="D43" t="s">
         <v>357</v>
       </c>
-      <c r="E43" t="e">
-        <v>#N/A</v>
+      <c r="E43" t="s">
+        <v>259</v>
       </c>
       <c r="F43" t="e">
         <v>#N/A</v>

</xml_diff>

<commit_message>
add xpath_new for Czech Republic
</commit_message>
<xml_diff>
--- a/manual/tests_urls.xlsx
+++ b/manual/tests_urls.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="469">
   <si>
     <t>country</t>
   </si>
@@ -1326,6 +1326,9 @@
   </si>
   <si>
     <t>(?&lt;=osoba, od toga)(.*)(?=u (protekla|posljednja) 24 sata)</t>
+  </si>
+  <si>
+    <t>/html/body/main/div[3]/div[1]/div[1]/div[1]/div/p[2]/span[2]</t>
   </si>
   <si>
     <t>//*[@id="top"]/div[2]/section[6]/div[1]/table/tbody/tr[3]/td[3]</t>
@@ -1719,7 +1722,7 @@
         <v>#N/A</v>
       </c>
       <c r="J8" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="9">
@@ -1783,7 +1786,7 @@
         <v>#N/A</v>
       </c>
       <c r="J10" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
     </row>
     <row r="11">
@@ -1815,7 +1818,7 @@
         <v>#N/A</v>
       </c>
       <c r="J11" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="12">
@@ -1847,7 +1850,7 @@
         <v>#N/A</v>
       </c>
       <c r="J12" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row r="13">
@@ -1879,7 +1882,7 @@
         <v>#N/A</v>
       </c>
       <c r="J13" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="14">
@@ -2167,7 +2170,7 @@
         <v>#N/A</v>
       </c>
       <c r="J22" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
     </row>
     <row r="23">
@@ -2455,7 +2458,7 @@
         <v>#N/A</v>
       </c>
       <c r="J31" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
     <row r="32">
@@ -2615,7 +2618,7 @@
         <v>#N/A</v>
       </c>
       <c r="J36" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="37">
@@ -2743,7 +2746,7 @@
         <v>#N/A</v>
       </c>
       <c r="J40" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
     </row>
     <row r="41">
@@ -2807,7 +2810,7 @@
         <v>#N/A</v>
       </c>
       <c r="J42" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="43">
@@ -2832,14 +2835,14 @@
       <c r="G43" t="s">
         <v>401</v>
       </c>
-      <c r="H43" t="e">
-        <v>#N/A</v>
+      <c r="H43" t="s">
+        <v>438</v>
       </c>
       <c r="I43" t="e">
         <v>#N/A</v>
       </c>
       <c r="J43" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
     </row>
     <row r="44">
@@ -2897,7 +2900,7 @@
         <v>402</v>
       </c>
       <c r="H45" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="I45" t="e">
         <v>#N/A</v>
@@ -3095,7 +3098,7 @@
         <v>#N/A</v>
       </c>
       <c r="J51" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
     <row r="52">
@@ -3351,7 +3354,7 @@
         <v>#N/A</v>
       </c>
       <c r="J59" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
     </row>
     <row r="60">
@@ -3863,7 +3866,7 @@
         <v>#N/A</v>
       </c>
       <c r="J75" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
     </row>
     <row r="76">
@@ -3895,7 +3898,7 @@
         <v>#N/A</v>
       </c>
       <c r="J76" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="77">
@@ -3959,7 +3962,7 @@
         <v>#N/A</v>
       </c>
       <c r="J78" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="79">
@@ -4247,7 +4250,7 @@
         <v>#N/A</v>
       </c>
       <c r="J87" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="88">
@@ -4343,7 +4346,7 @@
         <v>#N/A</v>
       </c>
       <c r="J90" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
     </row>
     <row r="91">
@@ -4407,7 +4410,7 @@
         <v>#N/A</v>
       </c>
       <c r="J92" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="93">
@@ -4567,7 +4570,7 @@
         <v>#N/A</v>
       </c>
       <c r="J97" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
     </row>
     <row r="98">
@@ -4791,7 +4794,7 @@
         <v>#N/A</v>
       </c>
       <c r="J104" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
     </row>
     <row r="105">
@@ -5015,7 +5018,7 @@
         <v>#N/A</v>
       </c>
       <c r="J111" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
     </row>
     <row r="112">
@@ -5175,7 +5178,7 @@
         <v>#N/A</v>
       </c>
       <c r="J116" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="117">
@@ -5335,7 +5338,7 @@
         <v>#N/A</v>
       </c>
       <c r="J121" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
     </row>
     <row r="122">
@@ -5393,7 +5396,7 @@
         <v>418</v>
       </c>
       <c r="H123" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="I123" t="e">
         <v>#N/A</v>
@@ -5431,7 +5434,7 @@
         <v>#N/A</v>
       </c>
       <c r="J124" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
     </row>
     <row r="125">
@@ -5553,7 +5556,7 @@
         <v>#N/A</v>
       </c>
       <c r="H128" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="I128" t="e">
         <v>#N/A</v>
@@ -5591,7 +5594,7 @@
         <v>#N/A</v>
       </c>
       <c r="J129" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
     </row>
     <row r="130">
@@ -5975,7 +5978,7 @@
         <v>#N/A</v>
       </c>
       <c r="J141" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
     </row>
     <row r="142">
@@ -6167,7 +6170,7 @@
         <v>#N/A</v>
       </c>
       <c r="J147" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="148">
@@ -6199,7 +6202,7 @@
         <v>#N/A</v>
       </c>
       <c r="J148" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
     </row>
     <row r="149">
@@ -6231,7 +6234,7 @@
         <v>#N/A</v>
       </c>
       <c r="J149" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="150">
@@ -6513,7 +6516,7 @@
         <v>428</v>
       </c>
       <c r="H158" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="I158" t="e">
         <v>#N/A</v>
@@ -6583,7 +6586,7 @@
         <v>#N/A</v>
       </c>
       <c r="J160" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
     </row>
     <row r="161">

</xml_diff>